<commit_message>
i# Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/Real_Estate_Valuation_Data_Set.xlsx
+++ b/Real_Estate_Valuation_Data_Set.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyanspatel/Desktop/Shreyans/PG_Work/CS6375_ML/Assignments/Assignment_1/Machine_Learning_Linear_Regression/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92F3D26-42D9-5B47-99EE-19F748386698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20016" windowHeight="9108"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20020" windowHeight="9100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,10 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
   <si>
     <t>X1 transaction date</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -57,19 +54,22 @@
     <t>Y house price of unit area</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>No</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -89,7 +89,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -163,13 +163,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -446,43 +446,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="8" width="30.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="8" width="30.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:8" ht="19">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">

</xml_diff>